<commit_message>
finished cataloging sql bugs, reorganized for cleaner directory
</commit_message>
<xml_diff>
--- a/bugs_table_sql.xlsx
+++ b/bugs_table_sql.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321B2558-EAC4-4E98-B910-665B4FB352F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976E37D1-67F4-4C72-9230-2AF51E567CD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>File</t>
   </si>
@@ -137,6 +137,54 @@
   </si>
   <si>
     <t>exprProbability(Expr *p)</t>
+  </si>
+  <si>
+    <t>sqlite3RowSetInsert(RowSet *p, i64 rowid)</t>
+  </si>
+  <si>
+    <t>pkg1/sqlite-3.21-buggy/src/rowset.c</t>
+  </si>
+  <si>
+    <t>pkg1/sqlite-3.21-buggy/src/tokenize.c</t>
+  </si>
+  <si>
+    <t>sqlite3IsIdChar(u8 c)</t>
+  </si>
+  <si>
+    <t>sqlite3DropTriggerPtr(Parse *pParse, Trigger *pTrigger)</t>
+  </si>
+  <si>
+    <t>pkg1/sqlite-3.21-buggy/src/trigger.c</t>
+  </si>
+  <si>
+    <t>pkg1/sqlite-3.21-buggy/src/vdbeapi.c</t>
+  </si>
+  <si>
+    <t>sqlite3_result_error_code(sqlite3_context *pCtx, int errCode)</t>
+  </si>
+  <si>
+    <t>sqlite3_bind_zeroblob(sqlite3_stmt *pStmt, int i, int n)</t>
+  </si>
+  <si>
+    <t>pkg1/sqlite-3.21-buggy/src/vdbeaux.c</t>
+  </si>
+  <si>
+    <t>sqlite3VdbeReusable(Vdbe *p)</t>
+  </si>
+  <si>
+    <t>pkg1/sqlite-3.21-buggy/src/vdbesort.c</t>
+  </si>
+  <si>
+    <t>vdbePmaReaderSeek(SortSubtask *pTask, PmaReader *pReadr, SorterFile *pFile, i64 iOff)</t>
+  </si>
+  <si>
+    <t>sqlite3WalLimit(Wal *pWal, i64 iLimit)</t>
+  </si>
+  <si>
+    <t>pkg1/sqlite-3.21-buggy/src/where.c</t>
+  </si>
+  <si>
+    <t>sqlite3WhereIsSorted(WhereInfo *pWInfo)</t>
   </si>
 </sst>
 </file>
@@ -454,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,6 +763,105 @@
         <v>554</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32">
+        <v>3789</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>